<commit_message>
fix all warnings v0.1.43
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-ESAVIQuestionnaireResponse.xlsx
+++ b/docs/StructureDefinition-ESAVIQuestionnaireResponse.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.42</t>
+    <t>0.1.43</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-01-16T11:37:21-03:00</t>
+    <t>2024-01-16T11:42:34-03:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>